<commit_message>
uniformity test, tester fix
</commit_message>
<xml_diff>
--- a/Analyzer Results/RESULTS_MERGED_DATE.xlsx
+++ b/Analyzer Results/RESULTS_MERGED_DATE.xlsx
@@ -511,16 +511,16 @@
         <v>21.73333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1128906152689321</v>
+        <v>74.25</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1317423792936151</v>
+        <v>20.153</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9094539716917553</v>
+        <v>174.8763333333333</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1514750540819768</v>
+        <v>8264.576999999999</v>
       </c>
     </row>
     <row r="3">
@@ -549,16 +549,16 @@
         <v>18.83333333333333</v>
       </c>
       <c r="G3" t="n">
-        <v>0.09955959285491885</v>
+        <v>72.01666666666667</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1119624234665848</v>
+        <v>19.37116666666667</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8614416338817082</v>
+        <v>167.1315</v>
       </c>
       <c r="J3" t="n">
-        <v>0.13987311322494</v>
+        <v>8111.620833333333</v>
       </c>
     </row>
     <row r="4">
@@ -587,16 +587,16 @@
         <v>20.73333333333333</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1495500281503433</v>
+        <v>79.75</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1920702489266754</v>
+        <v>22.2285</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8180105038466725</v>
+        <v>161.7388333333333</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2375300252844549</v>
+        <v>9261.135833333334</v>
       </c>
     </row>
     <row r="5">
@@ -625,16 +625,16 @@
         <v>18.8</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1605650498576471</v>
+        <v>81.26666666666667</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1985155646190523</v>
+        <v>22.43133333333333</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9223502842653298</v>
+        <v>177.5133333333333</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2698655208761866</v>
+        <v>9596.530000000001</v>
       </c>
     </row>
     <row r="6">
@@ -663,16 +663,16 @@
         <v>18.93333333333333</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1549503398879787</v>
+        <v>80.5</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1865922807380001</v>
+        <v>22.05383333333333</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8270203579284676</v>
+        <v>162.7735</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2329866016802497</v>
+        <v>9212.772500000001</v>
       </c>
     </row>
     <row r="7">
@@ -701,16 +701,16 @@
         <v>18.53333333333333</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1503840066797708</v>
+        <v>79.86666666666666</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1802865378658743</v>
+        <v>21.85</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8388122327374511</v>
+        <v>164.188</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2357126332053459</v>
+        <v>9241.831333333334</v>
       </c>
     </row>
     <row r="8">
@@ -739,16 +739,16 @@
         <v>18.36666666666667</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1205391682725363</v>
+        <v>75.46666666666667</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1619413515561778</v>
+        <v>21.238</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8760499036077235</v>
+        <v>169.2303333333333</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2409566647216229</v>
+        <v>9297.389000000001</v>
       </c>
     </row>
     <row r="9">
@@ -777,16 +777,16 @@
         <v>18.8</v>
       </c>
       <c r="G9" t="n">
-        <v>0.06206514654411289</v>
+        <v>64.60000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>0.06748589648453651</v>
+        <v>17.26333333333333</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8778725751543807</v>
+        <v>169.5053333333333</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0908599538307569</v>
+        <v>7373.910666666667</v>
       </c>
     </row>
     <row r="10">
@@ -815,16 +815,16 @@
         <v>26.8</v>
       </c>
       <c r="G10" t="n">
-        <v>0.02389880609584044</v>
+        <v>53</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02815002278605889</v>
+        <v>14.43733333333333</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9572956824757393</v>
+        <v>187.152</v>
       </c>
       <c r="J10" t="n">
-        <v>0.04202753575619969</v>
+        <v>6331.017333333333</v>
       </c>
     </row>
     <row r="11">
@@ -853,16 +853,16 @@
         <v>18.13333333333334</v>
       </c>
       <c r="G11" t="n">
-        <v>0.03227186092418627</v>
+        <v>56.26666666666666</v>
       </c>
       <c r="H11" t="n">
-        <v>0.03766147191751082</v>
+        <v>15.288</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9151798411529236</v>
+        <v>176.0066666666667</v>
       </c>
       <c r="J11" t="n">
-        <v>0.05148342371011796</v>
+        <v>6578.642</v>
       </c>
     </row>
     <row r="12">
@@ -891,16 +891,16 @@
         <v>19.6</v>
       </c>
       <c r="G12" t="n">
-        <v>0.04038391586664065</v>
+        <v>58.91666666666666</v>
       </c>
       <c r="H12" t="n">
-        <v>0.04429811508609683</v>
+        <v>15.79816666666667</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9436347449218436</v>
+        <v>182.7893333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>0.06011947232279832</v>
+        <v>6779.659</v>
       </c>
     </row>
     <row r="13">
@@ -929,16 +929,16 @@
         <v>19.63333333333333</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03554125913297194</v>
+        <v>57.38333333333333</v>
       </c>
       <c r="H13" t="n">
-        <v>0.03504827657034457</v>
+        <v>15.0705</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7753906146426808</v>
+        <v>157.2773333333333</v>
       </c>
       <c r="J13" t="n">
-        <v>0.04172283464004371</v>
+        <v>6322.440333333333</v>
       </c>
     </row>
     <row r="14">
@@ -967,16 +967,16 @@
         <v>18.93333333333333</v>
       </c>
       <c r="G14" t="n">
-        <v>0.04021944531900032</v>
+        <v>58.86666666666667</v>
       </c>
       <c r="H14" t="n">
-        <v>0.04463504292935868</v>
+        <v>15.82266666666666</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8704650761661021</v>
+        <v>168.4066666666666</v>
       </c>
       <c r="J14" t="n">
-        <v>0.05546560320404176</v>
+        <v>6673.869333333333</v>
       </c>
     </row>
     <row r="15">
@@ -1005,16 +1005,16 @@
         <v>18</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0853957805313552</v>
+        <v>69.45</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1135735377877701</v>
+        <v>19.4375</v>
       </c>
       <c r="I15" t="n">
-        <v>0.8931976066637436</v>
+        <v>171.9538333333333</v>
       </c>
       <c r="J15" t="n">
-        <v>0.171314386302811</v>
+        <v>8513.187333333333</v>
       </c>
     </row>
     <row r="16">
@@ -1043,16 +1043,16 @@
         <v>18.86666666666667</v>
       </c>
       <c r="G16" t="n">
-        <v>0.111761503048069</v>
+        <v>74.06666666666666</v>
       </c>
       <c r="H16" t="n">
-        <v>0.142460025252074</v>
+        <v>20.551</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8737370535562134</v>
+        <v>168.8858333333334</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2074809727989678</v>
+        <v>8934.2425</v>
       </c>
     </row>
     <row r="17">
@@ -1081,16 +1081,16 @@
         <v>16.73333333333333</v>
       </c>
       <c r="G17" t="n">
-        <v>0.03208340480832851</v>
+        <v>56.2</v>
       </c>
       <c r="H17" t="n">
-        <v>0.03776413329443399</v>
+        <v>15.29633333333333</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9501511878782898</v>
+        <v>184.7423333333333</v>
       </c>
       <c r="J17" t="n">
-        <v>0.05500394476934751</v>
+        <v>6663.064333333333</v>
       </c>
     </row>
     <row r="18">
@@ -1119,16 +1119,16 @@
         <v>18.93333333333333</v>
       </c>
       <c r="G18" t="n">
-        <v>0.03518964767662651</v>
+        <v>57.26666666666667</v>
       </c>
       <c r="H18" t="n">
-        <v>0.04234071519444245</v>
+        <v>15.65333333333333</v>
       </c>
       <c r="I18" t="n">
-        <v>0.831187622864662</v>
+        <v>163.2651666666667</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0688659717158424</v>
+        <v>6965.030833333333</v>
       </c>
     </row>
     <row r="19">
@@ -1157,16 +1157,16 @@
         <v>18</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03341844268206675</v>
+        <v>56.66666666666666</v>
       </c>
       <c r="H19" t="n">
-        <v>0.037039313028864</v>
+        <v>15.23716666666667</v>
       </c>
       <c r="I19" t="n">
-        <v>0.9297216724822366</v>
+        <v>179.1865</v>
       </c>
       <c r="J19" t="n">
-        <v>0.05463897901768779</v>
+        <v>6654.480333333333</v>
       </c>
     </row>
     <row r="20">
@@ -1195,16 +1195,16 @@
         <v>19.73333333333333</v>
       </c>
       <c r="G20" t="n">
-        <v>0.3273498029385503</v>
+        <v>100.6666666666667</v>
       </c>
       <c r="H20" t="n">
-        <v>0.4127411848539786</v>
+        <v>28.35466666666666</v>
       </c>
       <c r="I20" t="n">
-        <v>0.7886597491666903</v>
+        <v>158.5993333333333</v>
       </c>
       <c r="J20" t="n">
-        <v>0.5230742990019017</v>
+        <v>12035.004</v>
       </c>
     </row>
     <row r="21">
@@ -1233,16 +1233,16 @@
         <v>20.93333333333333</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3235774007148749</v>
+        <v>100.2666666666667</v>
       </c>
       <c r="H21" t="n">
-        <v>0.3642940022819451</v>
+        <v>27.082</v>
       </c>
       <c r="I21" t="n">
-        <v>0.5747159598092905</v>
+        <v>141.2246666666666</v>
       </c>
       <c r="J21" t="n">
-        <v>0.4115056081636654</v>
+        <v>10966.63866666667</v>
       </c>
     </row>
     <row r="22">
@@ -1271,16 +1271,16 @@
         <v>20.16666666666667</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3471096541800631</v>
+        <v>102.75</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4435474463664719</v>
+        <v>29.1645</v>
       </c>
       <c r="I22" t="n">
-        <v>0.8256426747149918</v>
+        <v>162.6128333333333</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5456130169742763</v>
+        <v>12258.31433333333</v>
       </c>
     </row>
     <row r="23">
@@ -1309,16 +1309,16 @@
         <v>20.23333333333333</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3243626807669306</v>
+        <v>100.35</v>
       </c>
       <c r="H23" t="n">
-        <v>0.425539742029493</v>
+        <v>28.69066666666667</v>
       </c>
       <c r="I23" t="n">
-        <v>0.8681310752733042</v>
+        <v>168.0705</v>
       </c>
       <c r="J23" t="n">
-        <v>0.5514814288502815</v>
+        <v>12317.11933333333</v>
       </c>
     </row>
     <row r="24">
@@ -1347,16 +1347,16 @@
         <v>21.06666666666667</v>
       </c>
       <c r="G24" t="n">
-        <v>0.4796458309497234</v>
+        <v>116.6</v>
       </c>
       <c r="H24" t="n">
-        <v>0.5798126774443402</v>
+        <v>32.88866666666667</v>
       </c>
       <c r="I24" t="n">
-        <v>0.7707510482749842</v>
+        <v>156.8273333333334</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6860564427880411</v>
+        <v>13783.62466666666</v>
       </c>
     </row>
     <row r="25">
@@ -1385,16 +1385,16 @@
         <v>23.06666666666667</v>
       </c>
       <c r="G25" t="n">
-        <v>0.3647811169572148</v>
+        <v>104.6</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4962642670495619</v>
+        <v>30.56733333333333</v>
       </c>
       <c r="I25" t="n">
-        <v>0.8668928511900128</v>
+        <v>167.894</v>
       </c>
       <c r="J25" t="n">
-        <v>0.6109200474433609</v>
+        <v>12932.40866666667</v>
       </c>
     </row>
     <row r="26">
@@ -1423,16 +1423,16 @@
         <v>20.93333333333333</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1720729617371289</v>
+        <v>82.8</v>
       </c>
       <c r="H26" t="n">
-        <v>0.210802540283962</v>
+        <v>22.81066666666667</v>
       </c>
       <c r="I26" t="n">
-        <v>0.8286436945036365</v>
+        <v>162.964</v>
       </c>
       <c r="J26" t="n">
-        <v>0.2786268161300962</v>
+        <v>9685.138666666668</v>
       </c>
     </row>
     <row r="27">
@@ -1461,16 +1461,16 @@
         <v>19.33333333333333</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2526803221769698</v>
+        <v>92.53333333333335</v>
       </c>
       <c r="H27" t="n">
-        <v>0.3179546605416368</v>
+        <v>25.84933333333333</v>
       </c>
       <c r="I27" t="n">
-        <v>0.8819185502189179</v>
+        <v>170.1273333333333</v>
       </c>
       <c r="J27" t="n">
-        <v>0.4160339375646716</v>
+        <v>11009.43333333333</v>
       </c>
     </row>
     <row r="28">
@@ -1499,16 +1499,16 @@
         <v>20.4</v>
       </c>
       <c r="G28" t="n">
-        <v>0.2805592135865405</v>
+        <v>95.63333333333333</v>
       </c>
       <c r="H28" t="n">
-        <v>0.3434784792579617</v>
+        <v>26.53133333333333</v>
       </c>
       <c r="I28" t="n">
-        <v>0.8496977432557631</v>
+        <v>165.5626666666667</v>
       </c>
       <c r="J28" t="n">
-        <v>0.4421585599396903</v>
+        <v>11256.62216666667</v>
       </c>
     </row>
     <row r="29">
@@ -1537,16 +1537,16 @@
         <v>20.3</v>
       </c>
       <c r="G29" t="n">
-        <v>0.2612814381101844</v>
+        <v>93.5</v>
       </c>
       <c r="H29" t="n">
-        <v>0.2728352278654895</v>
+        <v>24.61433333333333</v>
       </c>
       <c r="I29" t="n">
-        <v>0.6221979774656516</v>
+        <v>144.5983333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>0.2844459021399096</v>
+        <v>9743.541333333333</v>
       </c>
     </row>
     <row r="30">
@@ -1575,16 +1575,16 @@
         <v>19.46666666666667</v>
       </c>
       <c r="G30" t="n">
-        <v>0.2037311501210275</v>
+        <v>86.8</v>
       </c>
       <c r="H30" t="n">
-        <v>0.2320857009939933</v>
+        <v>23.448</v>
       </c>
       <c r="I30" t="n">
-        <v>0.75571812318626</v>
+        <v>155.4086666666667</v>
       </c>
       <c r="J30" t="n">
-        <v>0.3026474770540994</v>
+        <v>9924.168</v>
       </c>
     </row>
     <row r="31">
@@ -1613,16 +1613,16 @@
         <v>20.13333333333333</v>
       </c>
       <c r="G31" t="n">
-        <v>0.325305463596414</v>
+        <v>100.45</v>
       </c>
       <c r="H31" t="n">
-        <v>0.3890340827145466</v>
+        <v>27.73266666666667</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8444465592768082</v>
+        <v>164.8906666666667</v>
       </c>
       <c r="J31" t="n">
-        <v>0.4830658609934735</v>
+        <v>11646.63833333333</v>
       </c>
     </row>
     <row r="32">
@@ -1651,16 +1651,16 @@
         <v>20.13333333333334</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1945329033889045</v>
+        <v>85.66666666666667</v>
       </c>
       <c r="H32" t="n">
-        <v>0.2515018670828351</v>
+        <v>24.01133333333333</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9246019962314513</v>
+        <v>178.01</v>
       </c>
       <c r="J32" t="n">
-        <v>0.3300571979889609</v>
+        <v>10191.37066666667</v>
       </c>
     </row>
     <row r="33">
@@ -1689,16 +1689,16 @@
         <v>20.4</v>
       </c>
       <c r="G33" t="n">
-        <v>0.2741912913439757</v>
+        <v>94.93333333333334</v>
       </c>
       <c r="H33" t="n">
-        <v>0.3156398590676749</v>
+        <v>25.787</v>
       </c>
       <c r="I33" t="n">
-        <v>0.7532611963240694</v>
+        <v>155.1821666666667</v>
       </c>
       <c r="J33" t="n">
-        <v>0.3882581306337493</v>
+        <v>10746.83216666667</v>
       </c>
     </row>
     <row r="34">
@@ -1727,16 +1727,16 @@
         <v>20.03333333333333</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2672636383353582</v>
+        <v>94.16666666666667</v>
       </c>
       <c r="H34" t="n">
-        <v>0.3093998851316103</v>
+        <v>25.6185</v>
       </c>
       <c r="I34" t="n">
-        <v>0.7035132064049718</v>
+        <v>150.8651666666667</v>
       </c>
       <c r="J34" t="n">
-        <v>0.3736633696838446</v>
+        <v>10608.5025</v>
       </c>
     </row>
     <row r="35">
@@ -1765,16 +1765,16 @@
         <v>19.55555555555556</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2299203900564728</v>
+        <v>89.92222222222222</v>
       </c>
       <c r="H35" t="n">
-        <v>0.2858030476015133</v>
+        <v>24.97416666666667</v>
       </c>
       <c r="I35" t="n">
-        <v>0.8085540711786029</v>
+        <v>160.6912222222222</v>
       </c>
       <c r="J35" t="n">
-        <v>0.3936300823598284</v>
+        <v>10797.66244444444</v>
       </c>
     </row>
     <row r="36">
@@ -1803,16 +1803,16 @@
         <v>20.93333333333333</v>
       </c>
       <c r="G36" t="n">
-        <v>0.2101879691133624</v>
+        <v>87.58333333333333</v>
       </c>
       <c r="H36" t="n">
-        <v>0.2625684344031408</v>
+        <v>24.326</v>
       </c>
       <c r="I36" t="n">
-        <v>0.8213749907716791</v>
+        <v>162.1208333333333</v>
       </c>
       <c r="J36" t="n">
-        <v>0.3397114229012357</v>
+        <v>10284.40516666667</v>
       </c>
     </row>
     <row r="37">
@@ -1841,16 +1841,16 @@
         <v>22.8</v>
       </c>
       <c r="G37" t="n">
-        <v>0.09491759536635808</v>
+        <v>71.2</v>
       </c>
       <c r="H37" t="n">
-        <v>0.113309555115219</v>
+        <v>19.42666666666667</v>
       </c>
       <c r="I37" t="n">
-        <v>0.8390774395701779</v>
+        <v>164.2206666666667</v>
       </c>
       <c r="J37" t="n">
-        <v>0.1466429206930511</v>
+        <v>8201.624666666668</v>
       </c>
     </row>
     <row r="38">
@@ -1879,16 +1879,16 @@
         <v>18.8</v>
       </c>
       <c r="G38" t="n">
-        <v>0.8952746811865711</v>
+        <v>180.8166666666667</v>
       </c>
       <c r="H38" t="n">
-        <v>0.8411561411558748</v>
+        <v>42.72733333333334</v>
       </c>
       <c r="I38" t="n">
-        <v>0.2914500787077696</v>
+        <v>122.0713333333333</v>
       </c>
       <c r="J38" t="n">
-        <v>0.7865447099554508</v>
+        <v>15152.64016666667</v>
       </c>
     </row>
     <row r="39">
@@ -1917,16 +1917,16 @@
         <v>21.46666666666667</v>
       </c>
       <c r="G39" t="n">
-        <v>0.950479288811987</v>
+        <v>203.9333333333333</v>
       </c>
       <c r="H39" t="n">
-        <v>0.9771920321896096</v>
+        <v>57.52266666666667</v>
       </c>
       <c r="I39" t="n">
-        <v>0.67021603234896</v>
+        <v>148.2046666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>0.989241192425814</v>
+        <v>23055.95</v>
       </c>
     </row>
     <row r="40">
@@ -1955,16 +1955,16 @@
         <v>21.6</v>
       </c>
       <c r="G40" t="n">
-        <v>0.9076523257084617</v>
+        <v>184.8666666666667</v>
       </c>
       <c r="H40" t="n">
-        <v>0.9273629441092396</v>
+        <v>49.144</v>
       </c>
       <c r="I40" t="n">
-        <v>0.5976215969905253</v>
+        <v>142.8326666666667</v>
       </c>
       <c r="J40" t="n">
-        <v>0.939323111343044</v>
+        <v>18851.46933333333</v>
       </c>
     </row>
     <row r="41">
@@ -1993,16 +1993,16 @@
         <v>20.2</v>
       </c>
       <c r="G41" t="n">
-        <v>0.8803369198585298</v>
+        <v>176.4333333333334</v>
       </c>
       <c r="H41" t="n">
-        <v>0.8918488787952933</v>
+        <v>45.98383333333334</v>
       </c>
       <c r="I41" t="n">
-        <v>0.6872702478717877</v>
+        <v>149.5481666666667</v>
       </c>
       <c r="J41" t="n">
-        <v>0.9240281721105073</v>
+        <v>18246.50333333333</v>
       </c>
     </row>
     <row r="42">
@@ -2031,16 +2031,16 @@
         <v>21.8</v>
       </c>
       <c r="G42" t="n">
-        <v>0.9076040537788966</v>
+        <v>184.85</v>
       </c>
       <c r="H42" t="n">
-        <v>0.9226177312806043</v>
+        <v>48.65366666666667</v>
       </c>
       <c r="I42" t="n">
-        <v>0.3865414159317912</v>
+        <v>128.6311666666667</v>
       </c>
       <c r="J42" t="n">
-        <v>0.9456212399179174</v>
+        <v>19140.04683333333</v>
       </c>
     </row>
     <row r="43">
@@ -2069,16 +2069,16 @@
         <v>20.8</v>
       </c>
       <c r="G43" t="n">
-        <v>0.939028781288338</v>
+        <v>197.7333333333333</v>
       </c>
       <c r="H43" t="n">
-        <v>0.9507267123775059</v>
+        <v>52.06666666666666</v>
       </c>
       <c r="I43" t="n">
-        <v>0.5519440362769664</v>
+        <v>139.6553333333333</v>
       </c>
       <c r="J43" t="n">
-        <v>0.9588301928597481</v>
+        <v>19856.204</v>
       </c>
     </row>
     <row r="44">
@@ -2107,16 +2107,16 @@
         <v>21.86666666666667</v>
       </c>
       <c r="G44" t="n">
-        <v>0.9269052019093491</v>
+        <v>192.2</v>
       </c>
       <c r="H44" t="n">
-        <v>0.9476968577273703</v>
+        <v>51.626</v>
       </c>
       <c r="I44" t="n">
-        <v>0.4526673256379372</v>
+        <v>133.0166666666667</v>
       </c>
       <c r="J44" t="n">
-        <v>0.9543982941035026</v>
+        <v>19595.70133333333</v>
       </c>
     </row>
     <row r="45">
@@ -2145,16 +2145,16 @@
         <v>22.33333333333333</v>
       </c>
       <c r="G45" t="n">
-        <v>0.714655274081599</v>
+        <v>144.6888888888889</v>
       </c>
       <c r="H45" t="n">
-        <v>0.7113150601980291</v>
+        <v>37.06788888888889</v>
       </c>
       <c r="I45" t="n">
-        <v>0.5273353816464206</v>
+        <v>137.9854444444444</v>
       </c>
       <c r="J45" t="n">
-        <v>0.7150867590390702</v>
+        <v>14144.708</v>
       </c>
     </row>
     <row r="46">
@@ -2183,16 +2183,16 @@
         <v>18.9</v>
       </c>
       <c r="G46" t="n">
-        <v>0.781751697662908</v>
+        <v>155.2166666666667</v>
       </c>
       <c r="H46" t="n">
-        <v>0.8115660244550011</v>
+        <v>41.197</v>
       </c>
       <c r="I46" t="n">
-        <v>0.5719915932684011</v>
+        <v>141.0355</v>
       </c>
       <c r="J46" t="n">
-        <v>0.8665931684374473</v>
+        <v>16637.5825</v>
       </c>
     </row>
     <row r="47">
@@ -2221,16 +2221,16 @@
         <v>19.86666666666667</v>
       </c>
       <c r="G47" t="n">
-        <v>0.815002850308682</v>
+        <v>161.3333333333333</v>
       </c>
       <c r="H47" t="n">
-        <v>0.8457403265091183</v>
+        <v>42.984</v>
       </c>
       <c r="I47" t="n">
-        <v>0.5721237473483162</v>
+        <v>141.0446666666666</v>
       </c>
       <c r="J47" t="n">
-        <v>0.8808109724581932</v>
+        <v>16972.12866666667</v>
       </c>
     </row>
     <row r="48">
@@ -2259,16 +2259,16 @@
         <v>18.83333333333333</v>
       </c>
       <c r="G48" t="n">
-        <v>0.847754873771941</v>
+        <v>168.25</v>
       </c>
       <c r="H48" t="n">
-        <v>0.8721802692951641</v>
+        <v>44.59666666666666</v>
       </c>
       <c r="I48" t="n">
-        <v>0.5324162312574616</v>
+        <v>138.3283333333333</v>
       </c>
       <c r="J48" t="n">
-        <v>0.912424089665781</v>
+        <v>17854.01333333333</v>
       </c>
     </row>
     <row r="49">
@@ -2297,16 +2297,16 @@
         <v>20.22222222222222</v>
       </c>
       <c r="G49" t="n">
-        <v>0.8533859190663758</v>
+        <v>169.5555555555555</v>
       </c>
       <c r="H49" t="n">
-        <v>0.8791177026619479</v>
+        <v>45.06444444444444</v>
       </c>
       <c r="I49" t="n">
-        <v>0.5560699383753025</v>
+        <v>139.9377777777778</v>
       </c>
       <c r="J49" t="n">
-        <v>0.9244896550831023</v>
+        <v>18263.14666666667</v>
       </c>
     </row>
     <row r="50">
@@ -2335,16 +2335,16 @@
         <v>18.66666666666667</v>
       </c>
       <c r="G50" t="n">
-        <v>0.7666557678609827</v>
+        <v>152.6666666666667</v>
       </c>
       <c r="H50" t="n">
-        <v>0.7841852129094273</v>
+        <v>39.93666666666667</v>
       </c>
       <c r="I50" t="n">
-        <v>0.7423681573960997</v>
+        <v>154.1946666666667</v>
       </c>
       <c r="J50" t="n">
-        <v>0.8216444615598714</v>
+        <v>15739.424</v>
       </c>
     </row>
     <row r="51">
@@ -2373,16 +2373,16 @@
         <v>20.93333333333333</v>
       </c>
       <c r="G51" t="n">
-        <v>0.822038445679053</v>
+        <v>162.7333333333333</v>
       </c>
       <c r="H51" t="n">
-        <v>0.7706744789556403</v>
+        <v>39.358</v>
       </c>
       <c r="I51" t="n">
-        <v>0.2178955873497474</v>
+        <v>116.4726666666667</v>
       </c>
       <c r="J51" t="n">
-        <v>0.7195798385686629</v>
+        <v>14202.66066666666</v>
       </c>
     </row>
     <row r="52">
@@ -2411,16 +2411,16 @@
         <v>20.1</v>
       </c>
       <c r="G52" t="n">
-        <v>0.8431019141584031</v>
+        <v>167.2</v>
       </c>
       <c r="H52" t="n">
-        <v>0.8738552834916538</v>
+        <v>44.70766666666666</v>
       </c>
       <c r="I52" t="n">
-        <v>0.6513457445610894</v>
+        <v>146.7591666666667</v>
       </c>
       <c r="J52" t="n">
-        <v>0.9196480814268078</v>
+        <v>18092.70533333334</v>
       </c>
     </row>
     <row r="53">
@@ -2449,16 +2449,16 @@
         <v>18.2</v>
       </c>
       <c r="G53" t="n">
-        <v>0.8704791683074992</v>
+        <v>173.7833333333333</v>
       </c>
       <c r="H53" t="n">
-        <v>0.8981703974897111</v>
+        <v>46.47433333333333</v>
       </c>
       <c r="I53" t="n">
-        <v>0.2663371639633003</v>
+        <v>120.233</v>
       </c>
       <c r="J53" t="n">
-        <v>0.9472864663830085</v>
+        <v>19221.241</v>
       </c>
     </row>
     <row r="54">
@@ -2487,16 +2487,16 @@
         <v>22.5</v>
       </c>
       <c r="G54" t="n">
-        <v>0.8614610237907663</v>
+        <v>171.5</v>
       </c>
       <c r="H54" t="n">
-        <v>0.9187291822086308</v>
+        <v>48.27083333333334</v>
       </c>
       <c r="I54" t="n">
-        <v>0.6892607386462755</v>
+        <v>149.7075</v>
       </c>
       <c r="J54" t="n">
-        <v>0.9360688290587519</v>
+        <v>18712.48416666667</v>
       </c>
     </row>
     <row r="55">
@@ -2525,16 +2525,16 @@
         <v>19.86666666666666</v>
       </c>
       <c r="G55" t="n">
-        <v>0.8449863560140053</v>
+        <v>167.6222222222222</v>
       </c>
       <c r="H55" t="n">
-        <v>0.8532069217425591</v>
+        <v>43.41533333333333</v>
       </c>
       <c r="I55" t="n">
-        <v>0.4187315398167588</v>
+        <v>130.7726666666667</v>
       </c>
       <c r="J55" t="n">
-        <v>0.876669964944047</v>
+        <v>16871.48422222222</v>
       </c>
     </row>
     <row r="56">
@@ -2563,16 +2563,16 @@
         <v>23.6</v>
       </c>
       <c r="G56" t="n">
-        <v>0.9520263588820574</v>
+        <v>204.8666666666667</v>
       </c>
       <c r="H56" t="n">
-        <v>0.9644993202614159</v>
+        <v>54.438</v>
       </c>
       <c r="I56" t="n">
-        <v>0.3800437310868765</v>
+        <v>128.196</v>
       </c>
       <c r="J56" t="n">
-        <v>0.9544297843523643</v>
+        <v>19597.47133333333</v>
       </c>
     </row>
     <row r="57">
@@ -2601,16 +2601,16 @@
         <v>20.93333333333333</v>
       </c>
       <c r="G57" t="n">
-        <v>0.9303832735080674</v>
+        <v>193.7</v>
       </c>
       <c r="H57" t="n">
-        <v>0.9224867051790728</v>
+        <v>48.6405</v>
       </c>
       <c r="I57" t="n">
-        <v>0.2187902567686142</v>
+        <v>116.5453333333333</v>
       </c>
       <c r="J57" t="n">
-        <v>0.8927958668955679</v>
+        <v>17280.52833333333</v>
       </c>
     </row>
     <row r="58">
@@ -2639,16 +2639,16 @@
         <v>24.53333333333333</v>
       </c>
       <c r="G58" t="n">
-        <v>0.9188053895818256</v>
+        <v>188.9333333333333</v>
       </c>
       <c r="H58" t="n">
-        <v>0.9312607946498879</v>
+        <v>49.568</v>
       </c>
       <c r="I58" t="n">
-        <v>0.5220350605682446</v>
+        <v>137.6286666666667</v>
       </c>
       <c r="J58" t="n">
-        <v>0.9089281931212081</v>
+        <v>17744.45333333333</v>
       </c>
     </row>
     <row r="59">
@@ -2677,16 +2677,16 @@
         <v>21.64444444444445</v>
       </c>
       <c r="G59" t="n">
-        <v>0.8975616067756478</v>
+        <v>181.5333333333333</v>
       </c>
       <c r="H59" t="n">
-        <v>0.8879768904332143</v>
+        <v>45.69511111111111</v>
       </c>
       <c r="I59" t="n">
-        <v>0.1561313523438955</v>
+        <v>111.0271111111111</v>
       </c>
       <c r="J59" t="n">
-        <v>0.8224485321824488</v>
+        <v>15753.84777777778</v>
       </c>
     </row>
     <row r="60">
@@ -2715,16 +2715,16 @@
         <v>19.86666666666666</v>
       </c>
       <c r="G60" t="n">
-        <v>0.9367001725748362</v>
+        <v>196.6</v>
       </c>
       <c r="H60" t="n">
-        <v>0.9399048810533467</v>
+        <v>50.58866666666668</v>
       </c>
       <c r="I60" t="n">
-        <v>0.2650450644542683</v>
+        <v>120.1366666666667</v>
       </c>
       <c r="J60" t="n">
-        <v>0.9307240307241391</v>
+        <v>18497.02066666667</v>
       </c>
     </row>
     <row r="61">
@@ -2753,16 +2753,16 @@
         <v>26.66666666666667</v>
       </c>
       <c r="G61" t="n">
-        <v>0.9154178342835888</v>
+        <v>187.65</v>
       </c>
       <c r="H61" t="n">
-        <v>0.9378123132419829</v>
+        <v>50.33033333333333</v>
       </c>
       <c r="I61" t="n">
-        <v>0.4381343275436389</v>
+        <v>132.0563333333333</v>
       </c>
       <c r="J61" t="n">
-        <v>0.9155135918705807</v>
+        <v>17953.9655</v>
       </c>
     </row>
     <row r="62">
@@ -2791,16 +2791,16 @@
         <v>21.46666666666667</v>
       </c>
       <c r="G62" t="n">
-        <v>0.9367001725748362</v>
+        <v>196.6</v>
       </c>
       <c r="H62" t="n">
-        <v>0.9301765250820532</v>
+        <v>49.448</v>
       </c>
       <c r="I62" t="n">
-        <v>0.4311208701867552</v>
+        <v>131.5926666666667</v>
       </c>
       <c r="J62" t="n">
-        <v>0.9125512570715779</v>
+        <v>17858.068</v>
       </c>
     </row>
     <row r="63">
@@ -2829,16 +2829,16 @@
         <v>20.66666666666667</v>
       </c>
       <c r="G63" t="n">
-        <v>0.8870160653445691</v>
+        <v>178.3333333333333</v>
       </c>
       <c r="H63" t="n">
-        <v>0.8761641459837965</v>
+        <v>44.86266666666666</v>
       </c>
       <c r="I63" t="n">
-        <v>0.2910798970412391</v>
+        <v>122.0446666666667</v>
       </c>
       <c r="J63" t="n">
-        <v>0.84241587969374</v>
+        <v>16129.30133333333</v>
       </c>
     </row>
     <row r="64">
@@ -2867,16 +2867,16 @@
         <v>20.03333333333333</v>
       </c>
       <c r="G64" t="n">
-        <v>0.8903490723374254</v>
+        <v>179.3166666666667</v>
       </c>
       <c r="H64" t="n">
-        <v>0.8900101143287499</v>
+        <v>45.84566666666667</v>
       </c>
       <c r="I64" t="n">
-        <v>0.3480917522576725</v>
+        <v>126.0348333333333</v>
       </c>
       <c r="J64" t="n">
-        <v>0.8822118194427915</v>
+        <v>17006.8225</v>
       </c>
     </row>
     <row r="65">
@@ -2905,16 +2905,16 @@
         <v>21.6</v>
       </c>
       <c r="G65" t="n">
-        <v>0.9106973686252194</v>
+        <v>185.9333333333333</v>
       </c>
       <c r="H65" t="n">
-        <v>0.9127963995513771</v>
+        <v>47.716</v>
       </c>
       <c r="I65" t="n">
-        <v>0.3650984391217831</v>
+        <v>127.19</v>
       </c>
       <c r="J65" t="n">
-        <v>0.8897788450488141</v>
+        <v>17200.31466666667</v>
       </c>
     </row>
     <row r="66">
@@ -2943,16 +2943,16 @@
         <v>20.43333333333333</v>
       </c>
       <c r="G66" t="n">
-        <v>0.9003223515466193</v>
+        <v>182.4166666666667</v>
       </c>
       <c r="H66" t="n">
-        <v>0.8929017626765499</v>
+        <v>46.06383333333334</v>
       </c>
       <c r="I66" t="n">
-        <v>0.2308648956271115</v>
+        <v>117.5128333333333</v>
       </c>
       <c r="J66" t="n">
-        <v>0.8719045701950977</v>
+        <v>16759.01416666667</v>
       </c>
     </row>
     <row r="67">
@@ -2981,16 +2981,16 @@
         <v>20.66666666666667</v>
       </c>
       <c r="G67" t="n">
-        <v>0.8830703762746773</v>
+        <v>177.2</v>
       </c>
       <c r="H67" t="n">
-        <v>0.8866672351671119</v>
+        <v>45.59933333333333</v>
       </c>
       <c r="I67" t="n">
-        <v>0.3035686045255027</v>
+        <v>122.938</v>
       </c>
       <c r="J67" t="n">
-        <v>0.8627594334005547</v>
+        <v>16552.332</v>
       </c>
     </row>
     <row r="68">
@@ -3019,16 +3019,16 @@
         <v>19.2</v>
       </c>
       <c r="G68" t="n">
-        <v>0.8920671231759189</v>
+        <v>179.8333333333333</v>
       </c>
       <c r="H68" t="n">
-        <v>0.8876415675740961</v>
+        <v>45.6705</v>
       </c>
       <c r="I68" t="n">
-        <v>0.3441245686883029</v>
+        <v>125.7635</v>
       </c>
       <c r="J68" t="n">
-        <v>0.8817078577360771</v>
+        <v>16994.3025</v>
       </c>
     </row>
     <row r="69">
@@ -3057,16 +3057,16 @@
         <v>20.4</v>
       </c>
       <c r="G69" t="n">
-        <v>0.8806964296586294</v>
+        <v>176.5333333333333</v>
       </c>
       <c r="H69" t="n">
-        <v>0.8680403421878602</v>
+        <v>44.32733333333334</v>
       </c>
       <c r="I69" t="n">
-        <v>0.2467911625893013</v>
+        <v>118.7546666666667</v>
       </c>
       <c r="J69" t="n">
-        <v>0.8329408957455307</v>
+        <v>15946.816</v>
       </c>
     </row>
     <row r="70">
@@ -3095,16 +3095,16 @@
         <v>21.76666666666667</v>
       </c>
       <c r="G70" t="n">
-        <v>0.8959705614862831</v>
+        <v>181.0333333333333</v>
       </c>
       <c r="H70" t="n">
-        <v>0.8915997593758629</v>
+        <v>45.965</v>
       </c>
       <c r="I70" t="n">
-        <v>0.2032813041761232</v>
+        <v>115.2646666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>0.8574888282649126</v>
+        <v>16438.19133333333</v>
       </c>
     </row>
     <row r="71">
@@ -3133,16 +3133,16 @@
         <v>21.6</v>
       </c>
       <c r="G71" t="n">
-        <v>0.8984017508643527</v>
+        <v>181.8</v>
       </c>
       <c r="H71" t="n">
-        <v>0.8993415795290119</v>
+        <v>46.568</v>
       </c>
       <c r="I71" t="n">
-        <v>0.242599644035262</v>
+        <v>118.4313333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>0.8809270732389209</v>
+        <v>16974.99133333334</v>
       </c>
     </row>
     <row r="72">
@@ -3171,16 +3171,16 @@
         <v>19.46666666666667</v>
       </c>
       <c r="G72" t="n">
-        <v>0.873082745560297</v>
+        <v>174.4666666666667</v>
       </c>
       <c r="H72" t="n">
-        <v>0.8439520619136773</v>
+        <v>42.88316666666666</v>
       </c>
       <c r="I72" t="n">
-        <v>0.1277207466028409</v>
+        <v>108.116</v>
       </c>
       <c r="J72" t="n">
-        <v>0.7943606863720719</v>
+        <v>15276.7295</v>
       </c>
     </row>
     <row r="73">
@@ -3209,16 +3209,16 @@
         <v>21.13333333333333</v>
       </c>
       <c r="G73" t="n">
-        <v>0.7134529949318531</v>
+        <v>144.5166666666667</v>
       </c>
       <c r="H73" t="n">
-        <v>0.6613018967525508</v>
+        <v>35.36966666666667</v>
       </c>
       <c r="I73" t="n">
-        <v>0.3694345320193778</v>
+        <v>127.4826666666667</v>
       </c>
       <c r="J73" t="n">
-        <v>0.6373152937359521</v>
+        <v>13220.12483333333</v>
       </c>
     </row>
     <row r="74">
@@ -3247,16 +3247,16 @@
         <v>18.53333333333333</v>
       </c>
       <c r="G74" t="n">
-        <v>0.6325085421233083</v>
+        <v>133.8333333333333</v>
       </c>
       <c r="H74" t="n">
-        <v>0.456868808830976</v>
+        <v>29.51633333333334</v>
       </c>
       <c r="I74" t="n">
-        <v>0.02273499534521204</v>
+        <v>89.66549999999999</v>
       </c>
       <c r="J74" t="n">
-        <v>0.2558488343267092</v>
+        <v>9452.892833333333</v>
       </c>
     </row>
     <row r="75">
@@ -3285,16 +3285,16 @@
         <v>16.26666666666667</v>
       </c>
       <c r="G75" t="n">
-        <v>0.6278799998871625</v>
+        <v>133.2666666666667</v>
       </c>
       <c r="H75" t="n">
-        <v>0.5451590176069776</v>
+        <v>31.906</v>
       </c>
       <c r="I75" t="n">
-        <v>0.05375573860051216</v>
+        <v>97.72733333333333</v>
       </c>
       <c r="J75" t="n">
-        <v>0.4786745190327377</v>
+        <v>11604.49933333333</v>
       </c>
     </row>
     <row r="76">
@@ -3323,16 +3323,16 @@
         <v>16.56666666666667</v>
       </c>
       <c r="G76" t="n">
-        <v>0.474922151425764</v>
+        <v>116.1</v>
       </c>
       <c r="H76" t="n">
-        <v>0.3022980416489295</v>
+        <v>25.42583333333333</v>
       </c>
       <c r="I76" t="n">
-        <v>0.03621138644822459</v>
+        <v>93.81066666666668</v>
       </c>
       <c r="J76" t="n">
-        <v>0.1623817172622808</v>
+        <v>8403.084499999999</v>
       </c>
     </row>
     <row r="77">
@@ -3361,16 +3361,16 @@
         <v>19.4</v>
       </c>
       <c r="G77" t="n">
-        <v>0.478544575505172</v>
+        <v>116.4833333333333</v>
       </c>
       <c r="H77" t="n">
-        <v>0.3160295481583673</v>
+        <v>25.7975</v>
       </c>
       <c r="I77" t="n">
-        <v>0.09364908804165172</v>
+        <v>104.041</v>
       </c>
       <c r="J77" t="n">
-        <v>0.1743154748712116</v>
+        <v>8549.5645</v>
       </c>
     </row>
     <row r="78">
@@ -3399,16 +3399,16 @@
         <v>17.73333333333333</v>
       </c>
       <c r="G78" t="n">
-        <v>0.6464659841335595</v>
+        <v>135.5666666666667</v>
       </c>
       <c r="H78" t="n">
-        <v>0.5084779684117045</v>
+        <v>30.8975</v>
       </c>
       <c r="I78" t="n">
-        <v>0.04820005897244817</v>
+        <v>96.60416666666667</v>
       </c>
       <c r="J78" t="n">
-        <v>0.3594576744193778</v>
+        <v>10473.38233333333</v>
       </c>
     </row>
     <row r="79">
@@ -3437,16 +3437,16 @@
         <v>18.53333333333333</v>
       </c>
       <c r="G79" t="n">
-        <v>0.5749655779313168</v>
+        <v>127.0333333333333</v>
       </c>
       <c r="H79" t="n">
-        <v>0.4152309361403756</v>
+        <v>28.42</v>
       </c>
       <c r="I79" t="n">
-        <v>0.0642719180644977</v>
+        <v>99.64366666666666</v>
       </c>
       <c r="J79" t="n">
-        <v>0.2793639835937582</v>
+        <v>9692.556333333334</v>
       </c>
     </row>
     <row r="80">
@@ -3475,16 +3475,16 @@
         <v>16.26666666666667</v>
       </c>
       <c r="G80" t="n">
-        <v>0.6493791764325528</v>
+        <v>135.9333333333333</v>
       </c>
       <c r="H80" t="n">
-        <v>0.4861628424285867</v>
+        <v>30.296</v>
       </c>
       <c r="I80" t="n">
-        <v>0.01124283681147114</v>
+        <v>84.146</v>
       </c>
       <c r="J80" t="n">
-        <v>0.3051044582336101</v>
+        <v>9948.335333333334</v>
       </c>
     </row>
     <row r="81">
@@ -3513,16 +3513,16 @@
         <v>16.8</v>
       </c>
       <c r="G81" t="n">
-        <v>0.5151552174847822</v>
+        <v>120.4</v>
       </c>
       <c r="H81" t="n">
-        <v>0.3221966975002276</v>
+        <v>25.96333333333333</v>
       </c>
       <c r="I81" t="n">
-        <v>0.01326413541497974</v>
+        <v>85.372</v>
       </c>
       <c r="J81" t="n">
-        <v>0.1516702071253823</v>
+        <v>8267.098</v>
       </c>
     </row>
     <row r="82">
@@ -3551,16 +3551,16 @@
         <v>20.23333333333333</v>
       </c>
       <c r="G82" t="n">
-        <v>0.4682921282634674</v>
+        <v>115.4</v>
       </c>
       <c r="H82" t="n">
-        <v>0.3234328667789366</v>
+        <v>25.9965</v>
       </c>
       <c r="I82" t="n">
-        <v>0.02149669400723563</v>
+        <v>89.19600000000001</v>
       </c>
       <c r="J82" t="n">
-        <v>0.1712872050798319</v>
+        <v>8512.8565</v>
       </c>
     </row>
     <row r="83">
@@ -3589,16 +3589,16 @@
         <v>18.63333333333334</v>
       </c>
       <c r="G83" t="n">
-        <v>0.5020049889380916</v>
+        <v>118.9833333333333</v>
       </c>
       <c r="H83" t="n">
-        <v>0.3572595932405659</v>
+        <v>26.89633333333333</v>
       </c>
       <c r="I83" t="n">
-        <v>0.04024631878953901</v>
+        <v>94.81849999999999</v>
       </c>
       <c r="J83" t="n">
-        <v>0.2139244765289049</v>
+        <v>9005.830833333333</v>
       </c>
     </row>
     <row r="84">
@@ -3627,16 +3627,16 @@
         <v>15.96666666666667</v>
       </c>
       <c r="G84" t="n">
-        <v>0.3431441559603309</v>
+        <v>102.3333333333333</v>
       </c>
       <c r="H84" t="n">
-        <v>0.2522590181741072</v>
+        <v>24.033</v>
       </c>
       <c r="I84" t="n">
-        <v>0.116470350785554</v>
+        <v>106.8558333333333</v>
       </c>
       <c r="J84" t="n">
-        <v>0.2211425085601703</v>
+        <v>9085.001666666667</v>
       </c>
     </row>
     <row r="85">
@@ -3665,16 +3665,16 @@
         <v>19.26666666666667</v>
       </c>
       <c r="G85" t="n">
-        <v>0.5030921719745142</v>
+        <v>119.1</v>
       </c>
       <c r="H85" t="n">
-        <v>0.3695500986433998</v>
+        <v>27.2205</v>
       </c>
       <c r="I85" t="n">
-        <v>0.04925227524982568</v>
+        <v>96.82383333333333</v>
       </c>
       <c r="J85" t="n">
-        <v>0.2286731500312632</v>
+        <v>9166.532499999999</v>
       </c>
     </row>
     <row r="86">
@@ -3703,16 +3703,16 @@
         <v>16.76666666666667</v>
       </c>
       <c r="G86" t="n">
-        <v>0.5632057261099758</v>
+        <v>125.7</v>
       </c>
       <c r="H86" t="n">
-        <v>0.4095967462120305</v>
+        <v>28.27216666666666</v>
       </c>
       <c r="I86" t="n">
-        <v>0.03612426728195389</v>
+        <v>93.78800000000001</v>
       </c>
       <c r="J86" t="n">
-        <v>0.3033409401963021</v>
+        <v>9930.993833333334</v>
       </c>
     </row>
     <row r="87">
@@ -3741,16 +3741,16 @@
         <v>17.86666666666667</v>
       </c>
       <c r="G87" t="n">
-        <v>0.4701883498114365</v>
+        <v>115.6</v>
       </c>
       <c r="H87" t="n">
-        <v>0.3286666274502525</v>
+        <v>26.13666666666667</v>
       </c>
       <c r="I87" t="n">
-        <v>0.1457916859261496</v>
+        <v>110.0066666666667</v>
       </c>
       <c r="J87" t="n">
-        <v>0.2150981045842772</v>
+        <v>9018.775333333333</v>
       </c>
     </row>
     <row r="88">
@@ -3779,16 +3779,16 @@
         <v>18</v>
       </c>
       <c r="G88" t="n">
-        <v>0.4954668334566541</v>
+        <v>118.2833333333333</v>
       </c>
       <c r="H88" t="n">
-        <v>0.2609649661501803</v>
+        <v>24.28066666666667</v>
       </c>
       <c r="I88" t="n">
-        <v>0.007023466206449175</v>
+        <v>80.85816666666666</v>
       </c>
       <c r="J88" t="n">
-        <v>0.08218571775194616</v>
+        <v>7220.7835</v>
       </c>
     </row>
     <row r="89">
@@ -3817,16 +3817,16 @@
         <v>15.33333333333333</v>
       </c>
       <c r="G89" t="n">
-        <v>0.5740886157615881</v>
+        <v>126.9333333333333</v>
       </c>
       <c r="H89" t="n">
-        <v>0.4107084684756901</v>
+        <v>28.30133333333334</v>
       </c>
       <c r="I89" t="n">
-        <v>0.02521591397381882</v>
+        <v>90.54933333333332</v>
       </c>
       <c r="J89" t="n">
-        <v>0.3014863169049948</v>
+        <v>9912.729999999998</v>
       </c>
     </row>
     <row r="90">
@@ -3855,16 +3855,16 @@
         <v>18.4</v>
       </c>
       <c r="G90" t="n">
-        <v>0.4594240805237764</v>
+        <v>114.4666666666667</v>
       </c>
       <c r="H90" t="n">
-        <v>0.331935086611634</v>
+        <v>26.224</v>
       </c>
       <c r="I90" t="n">
-        <v>0.144839957934834</v>
+        <v>109.9106666666667</v>
       </c>
       <c r="J90" t="n">
-        <v>0.2497768651448698</v>
+        <v>9389.875333333333</v>
       </c>
     </row>
     <row r="91">
@@ -3893,16 +3893,16 @@
         <v>22.26666666666667</v>
       </c>
       <c r="G91" t="n">
-        <v>0.2416946442576379</v>
+        <v>91.28333333333335</v>
       </c>
       <c r="H91" t="n">
-        <v>0.14298230318579</v>
+        <v>20.57</v>
       </c>
       <c r="I91" t="n">
-        <v>0.155925378591913</v>
+        <v>111.0071666666667</v>
       </c>
       <c r="J91" t="n">
-        <v>0.09575440892125116</v>
+        <v>7456.479833333334</v>
       </c>
     </row>
     <row r="92">
@@ -3931,16 +3931,16 @@
         <v>22.93333333333333</v>
       </c>
       <c r="G92" t="n">
-        <v>0.5120713450706359</v>
+        <v>120.0666666666667</v>
       </c>
       <c r="H92" t="n">
-        <v>0.5988905970950154</v>
+        <v>33.44533333333333</v>
       </c>
       <c r="I92" t="n">
-        <v>0.6220652041889365</v>
+        <v>144.5886666666667</v>
       </c>
       <c r="J92" t="n">
-        <v>0.6089501135464588</v>
+        <v>12911.34333333333</v>
       </c>
     </row>
     <row r="93">
@@ -3969,16 +3969,16 @@
         <v>21.46666666666667</v>
       </c>
       <c r="G93" t="n">
-        <v>0.4701883498114363</v>
+        <v>115.6</v>
       </c>
       <c r="H93" t="n">
-        <v>0.5129124554333507</v>
+        <v>31.018</v>
       </c>
       <c r="I93" t="n">
-        <v>0.6170693443301055</v>
+        <v>144.226</v>
       </c>
       <c r="J93" t="n">
-        <v>0.5117048428216915</v>
+        <v>11923.71333333333</v>
       </c>
     </row>
     <row r="94">
@@ -4007,16 +4007,16 @@
         <v>20.66666666666667</v>
       </c>
       <c r="G94" t="n">
-        <v>0.3967899321570317</v>
+        <v>107.9333333333333</v>
       </c>
       <c r="H94" t="n">
-        <v>0.4301312516152964</v>
+        <v>28.81133333333333</v>
       </c>
       <c r="I94" t="n">
-        <v>0.5459643707620887</v>
+        <v>139.2473333333333</v>
       </c>
       <c r="J94" t="n">
-        <v>0.414950994562769</v>
+        <v>10999.19866666667</v>
       </c>
     </row>
     <row r="95">
@@ -4045,16 +4045,16 @@
         <v>21.6</v>
       </c>
       <c r="G95" t="n">
-        <v>0.4971816590185664</v>
+        <v>118.4666666666667</v>
       </c>
       <c r="H95" t="n">
-        <v>0.5557202646811215</v>
+        <v>32.202</v>
       </c>
       <c r="I95" t="n">
-        <v>0.7223019862562829</v>
+        <v>152.4406666666667</v>
       </c>
       <c r="J95" t="n">
-        <v>0.5758920758911485</v>
+        <v>12565.132</v>
       </c>
     </row>
     <row r="96">
@@ -4083,16 +4083,16 @@
         <v>18.73333333333333</v>
       </c>
       <c r="G96" t="n">
-        <v>0.4232295682995465</v>
+        <v>110.6833333333333</v>
       </c>
       <c r="H96" t="n">
-        <v>0.4563964387561572</v>
+        <v>29.50383333333333</v>
       </c>
       <c r="I96" t="n">
-        <v>0.5252975752486991</v>
+        <v>137.8481666666667</v>
       </c>
       <c r="J96" t="n">
-        <v>0.4604553512067595</v>
+        <v>11430.44066666667</v>
       </c>
     </row>
     <row r="97">
@@ -4121,16 +4121,16 @@
         <v>19.33333333333333</v>
       </c>
       <c r="G97" t="n">
-        <v>0.4243499235241928</v>
+        <v>110.8</v>
       </c>
       <c r="H97" t="n">
-        <v>0.4223924708531777</v>
+        <v>28.608</v>
       </c>
       <c r="I97" t="n">
-        <v>0.4618056018387846</v>
+        <v>133.6206666666667</v>
       </c>
       <c r="J97" t="n">
-        <v>0.4100426965556823</v>
+        <v>10952.814</v>
       </c>
     </row>
     <row r="98">
@@ -4159,16 +4159,16 @@
         <v>20.66666666666667</v>
       </c>
       <c r="G98" t="n">
-        <v>0.4368195422328837</v>
+        <v>112.1</v>
       </c>
       <c r="H98" t="n">
-        <v>0.4749841452063226</v>
+        <v>29.99733333333333</v>
       </c>
       <c r="I98" t="n">
-        <v>0.5096379661729059</v>
+        <v>136.7975</v>
       </c>
       <c r="J98" t="n">
-        <v>0.4639978582061003</v>
+        <v>11464.19683333333</v>
       </c>
     </row>
     <row r="99">
@@ -4197,16 +4197,16 @@
         <v>20.13333333333333</v>
       </c>
       <c r="G99" t="n">
-        <v>0.3513989658425328</v>
+        <v>103.2</v>
       </c>
       <c r="H99" t="n">
-        <v>0.3573983704505815</v>
+        <v>26.9</v>
       </c>
       <c r="I99" t="n">
-        <v>0.545768576409535</v>
+        <v>139.234</v>
       </c>
       <c r="J99" t="n">
-        <v>0.3494771946935544</v>
+        <v>10378.06266666667</v>
       </c>
     </row>
     <row r="100">
@@ -4235,16 +4235,16 @@
         <v>20.93333333333333</v>
       </c>
       <c r="G100" t="n">
-        <v>0.3469509186725766</v>
+        <v>102.7333333333333</v>
       </c>
       <c r="H100" t="n">
-        <v>0.361311787185976</v>
+        <v>27.00333333333333</v>
       </c>
       <c r="I100" t="n">
-        <v>0.5481849682481268</v>
+        <v>139.3986666666667</v>
       </c>
       <c r="J100" t="n">
-        <v>0.3475087819096023</v>
+        <v>10359.218</v>
       </c>
     </row>
     <row r="101">
@@ -4273,16 +4273,16 @@
         <v>19.33333333333333</v>
       </c>
       <c r="G101" t="n">
-        <v>0.3387103142314641</v>
+        <v>101.8666666666667</v>
       </c>
       <c r="H101" t="n">
-        <v>0.3398661992367727</v>
+        <v>26.43533333333333</v>
       </c>
       <c r="I101" t="n">
-        <v>0.4490856608512201</v>
+        <v>132.78</v>
       </c>
       <c r="J101" t="n">
-        <v>0.3331953826364431</v>
+        <v>10221.66533333333</v>
       </c>
     </row>
     <row r="102">
@@ -4311,16 +4311,16 @@
         <v>20.66666666666667</v>
       </c>
       <c r="G102" t="n">
-        <v>0.3814086236892362</v>
+        <v>106.3333333333333</v>
       </c>
       <c r="H102" t="n">
-        <v>0.3992217577233209</v>
+        <v>28</v>
       </c>
       <c r="I102" t="n">
-        <v>0.5580168816620352</v>
+        <v>140.0713333333333</v>
       </c>
       <c r="J102" t="n">
-        <v>0.3933562272239471</v>
+        <v>10795.072</v>
       </c>
     </row>
     <row r="103">
@@ -4349,16 +4349,16 @@
         <v>21.33333333333333</v>
       </c>
       <c r="G103" t="n">
-        <v>0.3200218121135298</v>
+        <v>99.8888888888889</v>
       </c>
       <c r="H103" t="n">
-        <v>0.3315023017106985</v>
+        <v>26.21244444444445</v>
       </c>
       <c r="I103" t="n">
-        <v>0.4472863570916368</v>
+        <v>132.6611111111111</v>
       </c>
       <c r="J103" t="n">
-        <v>0.3086208371334548</v>
+        <v>9982.842444444444</v>
       </c>
     </row>
     <row r="104">
@@ -4387,16 +4387,16 @@
         <v>19.36666666666667</v>
       </c>
       <c r="G104" t="n">
-        <v>0.4288294290749756</v>
+        <v>111.2666666666667</v>
       </c>
       <c r="H104" t="n">
-        <v>0.4376195706249518</v>
+        <v>29.00833333333334</v>
       </c>
       <c r="I104" t="n">
-        <v>0.5195768479507696</v>
+        <v>137.4635</v>
       </c>
       <c r="J104" t="n">
-        <v>0.4355545643418257</v>
+        <v>11194.05683333333</v>
       </c>
     </row>
     <row r="105">
@@ -4425,16 +4425,16 @@
         <v>19.73333333333333</v>
       </c>
       <c r="G105" t="n">
-        <v>0.3471096541800631</v>
+        <v>102.75</v>
       </c>
       <c r="H105" t="n">
-        <v>0.3470459351086155</v>
+        <v>26.626</v>
       </c>
       <c r="I105" t="n">
-        <v>0.4896385572093589</v>
+        <v>135.4646666666667</v>
       </c>
       <c r="J105" t="n">
-        <v>0.3387041796958929</v>
+        <v>10274.72066666667</v>
       </c>
     </row>
     <row r="106">
@@ -4463,16 +4463,16 @@
         <v>19.33333333333333</v>
       </c>
       <c r="G106" t="n">
-        <v>0.3587208370627614</v>
+        <v>103.9666666666667</v>
       </c>
       <c r="H106" t="n">
-        <v>0.3734884569752933</v>
+        <v>27.32416666666667</v>
       </c>
       <c r="I106" t="n">
-        <v>0.5669186262159964</v>
+        <v>140.6843333333333</v>
       </c>
       <c r="J106" t="n">
-        <v>0.3752744167091082</v>
+        <v>10623.79283333333</v>
       </c>
     </row>
     <row r="107">
@@ -4501,16 +4501,16 @@
         <v>19.8</v>
       </c>
       <c r="G107" t="n">
-        <v>0.2878838657632519</v>
+        <v>96.43333333333334</v>
       </c>
       <c r="H107" t="n">
-        <v>0.2854706905674971</v>
+        <v>24.965</v>
       </c>
       <c r="I107" t="n">
-        <v>0.5147841815731116</v>
+        <v>137.142</v>
       </c>
       <c r="J107" t="n">
-        <v>0.2836436794268108</v>
+        <v>9735.510166666667</v>
       </c>
     </row>
     <row r="108">
@@ -4539,16 +4539,16 @@
         <v>19.46666666666667</v>
       </c>
       <c r="G108" t="n">
-        <v>0.336812677275533</v>
+        <v>101.6666666666667</v>
       </c>
       <c r="H108" t="n">
-        <v>0.3182272109679658</v>
+        <v>25.85666666666667</v>
       </c>
       <c r="I108" t="n">
-        <v>0.3995337627070585</v>
+        <v>129.498</v>
       </c>
       <c r="J108" t="n">
-        <v>0.2882728399824835</v>
+        <v>9781.767333333333</v>
       </c>
     </row>
     <row r="109">
@@ -4577,16 +4577,16 @@
         <v>20.23333333333333</v>
       </c>
       <c r="G109" t="n">
-        <v>0.1189456248745838</v>
+        <v>75.21666666666667</v>
       </c>
       <c r="H109" t="n">
-        <v>0.09669268224068453</v>
+        <v>18.71416666666667</v>
       </c>
       <c r="I109" t="n">
-        <v>0.5553849745796717</v>
+        <v>139.8908333333333</v>
       </c>
       <c r="J109" t="n">
-        <v>0.088527345163843</v>
+        <v>7333.629166666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>